<commit_message>
Ready for component addition
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299CEE7F-1A19-417B-ABD2-C327BBB10E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3BC72-6CCB-4B53-9BD2-2DC895C65A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Description</t>
   </si>
@@ -52,31 +52,16 @@
     <t>N1</t>
   </si>
   <si>
-    <t>The product will fit a circular floor drain.</t>
-  </si>
-  <si>
     <t>N2</t>
   </si>
   <si>
-    <t>The product prevents back flow of water.</t>
-  </si>
-  <si>
     <t>N3</t>
   </si>
   <si>
-    <t>The product will easy to install, quick to install, and can be installed without tools.</t>
-  </si>
-  <si>
     <t>N4</t>
   </si>
   <si>
-    <t>The activation force of the product will be reasonable for people with moderate hand strength and limited dexterity.</t>
-  </si>
-  <si>
     <t>N5</t>
-  </si>
-  <si>
-    <t>The product will minimize tripping hazard.</t>
   </si>
   <si>
     <t>Workflow</t>
@@ -883,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63EEA10-09B8-4C73-AD25-44735EA2ECAA}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,45 +954,30 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1015,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1023,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1031,27 +1001,27 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1059,50 +1029,52 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C26" s="12">
         <f>[1]Structural!$D$5</f>
         <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C27" s="12">
         <f>[1]Structural!$D$6</f>
         <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C28" s="12">
         <f>[1]Structural!$D$7</f>
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1110,16 +1082,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1163,21 +1135,21 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C42" s="4"/>
     </row>
@@ -1320,7 +1292,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1328,74 +1300,74 @@
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7">
         <f>'Overview and Inputs'!C26*2</f>
         <v>142</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7">
         <f>'Overview and Inputs'!C27*2</f>
         <v>136</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7">
         <f>'Overview and Inputs'!C28</f>
         <v>50</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>25</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1441,7 +1413,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1449,112 +1421,112 @@
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1">
         <v>200</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7">
         <f>'Nose Cone'!B4-Ribcage!B3*2</f>
         <v>126</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="7">
         <f>'Nose Cone'!B6</f>
         <v>25</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1">
         <v>15</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed length of body
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB7484E-853A-4CAD-8420-08CBC444B9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F725821F-33D0-4518-8978-BCDEEE6D4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -286,7 +286,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +376,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -403,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -438,6 +445,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,7 +1427,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,8 +1476,8 @@
         <v>19</v>
       </c>
       <c r="B4" s="7">
-        <f>'Overview and Inputs'!C27*2</f>
-        <v>136</v>
+        <f>'Overview and Inputs'!C27*2-1</f>
+        <v>135</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -1479,7 +1487,7 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="18">
         <f>'Overview and Inputs'!C28</f>
         <v>50</v>
       </c>
@@ -1547,7 +1555,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1596,7 +1604,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="1">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -1608,7 +1616,7 @@
       </c>
       <c r="B5" s="7">
         <f>'Nose Cone'!B4-Ribcage!B3*2</f>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -1942,7 +1950,7 @@
       </c>
       <c r="B3" s="7">
         <f>Ribcage!B5</f>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -1954,7 +1962,7 @@
       </c>
       <c r="B4" s="7">
         <f>Table42[[#This Row],[Value]]</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2263,7 +2271,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>131.80000000000001</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2297,7 +2305,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>55.900000000000006</v>
+        <v>55.400000000000006</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2320,7 +2328,7 @@
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>55.900000000000006</v>
+        <v>55.400000000000006</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
linking nose cone to spreadsheet
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F725821F-33D0-4518-8978-BCDEEE6D4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4128B7D-121E-45F9-B254-8FCE5023B42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Ribcage" sheetId="5" r:id="rId3"/>
     <sheet name="Shell" sheetId="7" r:id="rId4"/>
     <sheet name="Bulkhead" sheetId="8" r:id="rId5"/>
+    <sheet name="Arm Wheel &amp; Arm" sheetId="11" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -254,9 +255,6 @@
     <t>Diameter</t>
   </si>
   <si>
-    <t>Separatoin from Nose Cone</t>
-  </si>
-  <si>
     <t>Thickness</t>
   </si>
   <si>
@@ -276,6 +274,48 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Separation from Nose Cone</t>
+  </si>
+  <si>
+    <t>Arm Extension Angle</t>
+  </si>
+  <si>
+    <t>Arm Stop Angle</t>
+  </si>
+  <si>
+    <t>Pitot Hole Diameter</t>
+  </si>
+  <si>
+    <t>Pitot tube is 4.17mm in diam, ample toleance given.</t>
+  </si>
+  <si>
+    <t>Rod Thickness</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>Arm Cutout Width</t>
+  </si>
+  <si>
+    <t>Arm Cutout Tolerance</t>
+  </si>
+  <si>
+    <t>Arm Hinge Width</t>
+  </si>
+  <si>
+    <t>Wheel Diameter</t>
+  </si>
+  <si>
+    <t>Arm Holder Length</t>
+  </si>
+  <si>
+    <t>Arm Holder Width</t>
+  </si>
+  <si>
+    <t>Arm Wheel &amp; Arm</t>
   </si>
 </sst>
 </file>
@@ -286,7 +326,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,13 +416,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,12 +478,47 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -606,7 +674,7 @@
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{BF4FBE53-75C8-484D-9478-97DF7393A1CC}"/>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{677D2D52-0B6C-4B16-81C9-28445C0D9EA5}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -669,8 +737,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5847D800-2737-4C4E-8650-CB8B550670C6}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{30BDBAD9-10CB-40CA-8069-09092D99504D}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -682,8 +750,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A9055BBA-1249-4E95-814E-26A0A5B1B66C}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{9C1D3036-3428-4217-BD9C-B256247B98EA}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -695,8 +763,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2AB09C10-555A-4FA5-825E-671C56C5204E}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{7AF4781C-1A05-4414-BB69-E3894335BB8B}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -708,9 +776,22 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0B1EF6EA-7B8F-43FA-94CF-9EC466EA2E42}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{59D44731-521A-4BFC-A838-854482140970}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{820F1844-C478-4F0E-AC9D-B64CCEBF3897}" name="Table42346" displayName="Table42346" ref="A2:D1048576" totalsRowShown="0">
+  <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{08ED45E6-44A0-4E17-968F-5621C3E7B4A1}" name="Dimension"/>
+    <tableColumn id="2" xr3:uid="{957D3AA8-B8AB-4AF6-865C-352EAE7F21BA}" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{99CBAB39-6963-4DDA-B437-CB2F3F8008D2}" name="Units" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{72EE9F42-A042-455C-9AEB-3FDF7CA75325}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1424,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1117B8E-EE6B-4EA3-984B-68AD88614518}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,7 +1568,7 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="7">
         <f>'Overview and Inputs'!C28</f>
         <v>50</v>
       </c>
@@ -1522,20 +1603,101 @@
         <v>47</v>
       </c>
       <c r="B8" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="7">
+        <f>'Arm Wheel &amp; Arm'!B3</f>
+        <v>40</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7">
+        <f>'Arm Wheel &amp; Arm'!B5+1</f>
+        <v>7.5</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1554,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC87B61D-89B4-4354-BE4D-52F1AB79BE0D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2221,7 +2383,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2256,10 +2418,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -2271,7 +2433,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>130.80000000000001</v>
+        <v>131.4</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2279,7 +2441,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -2290,7 +2452,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1">
         <v>10</v>
@@ -2301,11 +2463,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>55.400000000000006</v>
+        <v>55.7</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2313,7 +2475,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
@@ -2324,11 +2486,11 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>55.400000000000006</v>
+        <v>55.7</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>
@@ -2336,14 +2498,346 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
+  <dimension ref="A1:D80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="112.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
update egg holder with spreadsheet
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7898807-94FC-4682-8791-4D102619AAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDA36C4-5105-449D-87C2-8C2B3064F87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2380,7 +2380,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Small edits, added screws to nose cone
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDA36C4-5105-449D-87C2-8C2B3064F87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AEEBCF-DF2D-4F87-8D82-7225666ED086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="Shell" sheetId="7" r:id="rId4"/>
     <sheet name="Bulkhead" sheetId="8" r:id="rId5"/>
     <sheet name="Arm Wheel &amp; Arm" sheetId="11" r:id="rId6"/>
+    <sheet name="Electronics Board" sheetId="13" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -313,6 +314,9 @@
   </si>
   <si>
     <t>Rod Diameter</t>
+  </si>
+  <si>
+    <t>Electronics Board</t>
   </si>
 </sst>
 </file>
@@ -479,7 +483,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -671,7 +711,7 @@
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{BF4FBE53-75C8-484D-9478-97DF7393A1CC}"/>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{677D2D52-0B6C-4B16-81C9-28445C0D9EA5}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -734,8 +774,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5847D800-2737-4C4E-8650-CB8B550670C6}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{30BDBAD9-10CB-40CA-8069-09092D99504D}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -747,8 +787,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A9055BBA-1249-4E95-814E-26A0A5B1B66C}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{9C1D3036-3428-4217-BD9C-B256247B98EA}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -760,8 +800,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2AB09C10-555A-4FA5-825E-671C56C5204E}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{7AF4781C-1A05-4414-BB69-E3894335BB8B}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -773,8 +813,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0B1EF6EA-7B8F-43FA-94CF-9EC466EA2E42}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{59D44731-521A-4BFC-A838-854482140970}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -786,9 +826,22 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{08ED45E6-44A0-4E17-968F-5621C3E7B4A1}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{957D3AA8-B8AB-4AF6-865C-352EAE7F21BA}" name="Value" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{99CBAB39-6963-4DDA-B437-CB2F3F8008D2}" name="Units" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{957D3AA8-B8AB-4AF6-865C-352EAE7F21BA}" name="Value" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{99CBAB39-6963-4DDA-B437-CB2F3F8008D2}" name="Units" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{72EE9F42-A042-455C-9AEB-3FDF7CA75325}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22C88779-5574-4A47-B1A5-989F7D15AF94}" name="Table423467" displayName="Table423467" ref="A2:D1048576" totalsRowShown="0">
+  <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{875DCB20-9A5B-4AE5-9B86-9FAA788CBC89}" name="Dimension"/>
+    <tableColumn id="2" xr3:uid="{7B1A0CB3-1D6F-469F-9208-C86A05C85E0A}" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FB7EDCA0-CC79-4DF2-9D3C-281C141BCEF3}" name="Units" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B19EAADD-84D4-408B-B3B0-38E4F735B850}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2379,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F3E7A-7DA3-40B7-A994-AE85F749A01D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2730,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3056,4 +3109,288 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D816C7CA-793D-4BAF-98F3-443B8F117F52}">
+  <dimension ref="A1:D80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="112.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Springs are very real and I very hate them. they work now.
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AEEBCF-DF2D-4F87-8D82-7225666ED086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8202F48-18CE-48FF-AC75-A2BA5D14CFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -2432,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F3E7A-7DA3-40B7-A994-AE85F749A01D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
finalized egg protection, updated assembly
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8202F48-18CE-48FF-AC75-A2BA5D14CFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE56D8-AC41-4C14-BB08-98D8CC4E24F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="504" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -1767,7 +1767,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F3E7A-7DA3-40B7-A994-AE85F749A01D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New diameter just dropped
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE56D8-AC41-4C14-BB08-98D8CC4E24F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A7A5F-161E-45DB-99C2-36592F63DFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -1767,7 +1767,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,7 +1805,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B5" s="7">
         <f>'Nose Cone'!B4-Ribcage!B3*2</f>
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -1873,7 +1873,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="B3" s="7">
         <f>Ribcage!B5</f>
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -2433,7 +2433,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2471,7 +2471,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>131.4</v>
+        <v>121.4</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>55.7</v>
+        <v>50.7</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>55.7</v>
+        <v>50.7</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated electronics board and egg holder with new diameters
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A7A5F-161E-45DB-99C2-36592F63DFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD778C2-897A-44C3-BC74-41D3315D745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -2432,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F3E7A-7DA3-40B7-A994-AE85F749A01D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3115,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D816C7CA-793D-4BAF-98F3-443B8F117F52}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
testing configuration for nose cone
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD778C2-897A-44C3-BC74-41D3315D745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EF024F-6486-4B84-98F5-8963A8313BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2833,7 +2833,7 @@
         <v>69</v>
       </c>
       <c r="B4" s="1">
-        <v>3.18</v>
+        <v>4</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -3115,7 +3115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D816C7CA-793D-4BAF-98F3-443B8F117F52}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Meager updates to arm wheel
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EF024F-6486-4B84-98F5-8963A8313BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B79B97B-6209-4440-AC23-EBACD2459D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -1557,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1117B8E-EE6B-4EA3-984B-68AD88614518}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1653,7 +1653,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="1">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>26</v>
@@ -1690,7 +1690,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>26</v>
@@ -1701,8 +1701,8 @@
         <v>62</v>
       </c>
       <c r="B12" s="7">
-        <f>'Arm Wheel &amp; Arm'!B5+1</f>
-        <v>7</v>
+        <f>'Arm Wheel &amp; Arm'!B5+B11</f>
+        <v>6.25</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>26</v>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>121.4</v>
+        <v>119.80000000000001</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>50.7</v>
+        <v>49.900000000000006</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>50.7</v>
+        <v>49.900000000000006</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>
@@ -2783,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Assembly fixes, nose cone diameter edit
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B79B97B-6209-4440-AC23-EBACD2459D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2F8255-2EC1-4F07-9ED2-89FF7107260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>Electronics Board</t>
+  </si>
+  <si>
+    <t>Shoulder Diameter Tolerance</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1150,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,11 +1561,12 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="16.21875" style="14" customWidth="1"/>
     <col min="4" max="4" width="112.6640625" customWidth="1"/>
@@ -1607,8 +1611,8 @@
         <v>19</v>
       </c>
       <c r="B4" s="7">
-        <f>'Overview and Inputs'!C27*2-1</f>
-        <v>135</v>
+        <f>'Overview and Inputs'!C27*2-B14</f>
+        <v>135.5</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -1720,7 +1724,15 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
@@ -1828,7 +1840,7 @@
       </c>
       <c r="B5" s="7">
         <f>'Nose Cone'!B4-Ribcage!B3*2</f>
-        <v>95</v>
+        <v>95.5</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -2162,7 +2174,7 @@
       </c>
       <c r="B3" s="7">
         <f>Ribcage!B5</f>
-        <v>95</v>
+        <v>95.5</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -2483,7 +2495,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>119.80000000000001</v>
+        <v>120.30000000000001</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2517,7 +2529,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>49.900000000000006</v>
+        <v>50.150000000000006</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2540,7 +2552,7 @@
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>49.900000000000006</v>
+        <v>50.150000000000006</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
New pitot holder started
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2F8255-2EC1-4F07-9ED2-89FF7107260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F338B0DA-D140-4931-8B21-84E68ADA559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t>Description</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Shoulder Diameter Tolerance</t>
+  </si>
+  <si>
+    <t>Lip To Tip Height</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1564,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,7 +1738,16 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="7">
+        <f>B7+((B4/2)/TAN(RADIANS(B6)))-2</f>
+        <v>153.29034386452261</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>

</xml_diff>

<commit_message>
Tolerance edits, started working on gears
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F338B0DA-D140-4931-8B21-84E68ADA559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEAA4E-055F-4B1E-BF5B-82A5B9C1BDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,7 +1697,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="1">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>26</v>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B12" s="7">
         <f>'Arm Wheel &amp; Arm'!B5+B11</f>
-        <v>6.25</v>
+        <v>6.2</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added a dummy assembly to do weird designs to, added rocket body model and assem using it, made alternate designs, changed tolerances, made dimension drawings
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEAA4E-055F-4B1E-BF5B-82A5B9C1BDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A8E366-8D83-4F13-8211-DEB9EB7A35CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,8 +1614,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="7">
-        <f>'Overview and Inputs'!C27*2-B14</f>
-        <v>135.5</v>
+        <v>135</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -1743,7 +1742,7 @@
       </c>
       <c r="B15" s="7">
         <f>B7+((B4/2)/TAN(RADIANS(B6)))-2</f>
-        <v>153.29034386452261</v>
+        <v>152.75421713439522</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>26</v>
@@ -1852,7 +1851,7 @@
       </c>
       <c r="B5" s="7">
         <f>'Nose Cone'!B4-Ribcage!B3*2</f>
-        <v>95.5</v>
+        <v>95</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -2186,7 +2185,7 @@
       </c>
       <c r="B3" s="7">
         <f>Ribcage!B5</f>
-        <v>95.5</v>
+        <v>95</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
@@ -2507,7 +2506,7 @@
       </c>
       <c r="B4" s="7">
         <f>'Nose Cone'!B4-'Nose Cone'!B8*2-B3*2</f>
-        <v>120.30000000000001</v>
+        <v>119.80000000000001</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2541,7 +2540,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/2-B6</f>
-        <v>50.150000000000006</v>
+        <v>49.900000000000006</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>26</v>
@@ -2564,7 +2563,7 @@
       </c>
       <c r="B9" s="1">
         <f>B4/2-B8</f>
-        <v>50.150000000000006</v>
+        <v>49.900000000000006</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
this is not a folder of honor.
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A8E366-8D83-4F13-8211-DEB9EB7A35CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C888EA3-88E0-42B9-AAF8-CC752B71A1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" tabRatio="667" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -316,13 +316,19 @@
     <t>Rod Diameter</t>
   </si>
   <si>
-    <t>Electronics Board</t>
-  </si>
-  <si>
     <t>Shoulder Diameter Tolerance</t>
   </si>
   <si>
     <t>Lip To Tip Height</t>
+  </si>
+  <si>
+    <t>Battery and Camera Holders</t>
+  </si>
+  <si>
+    <t>Distance between threaded rods</t>
+  </si>
+  <si>
+    <t>Offset from board</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1117B8E-EE6B-4EA3-984B-68AD88614518}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1727,7 +1733,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1">
         <v>0.5</v>
@@ -1738,7 +1744,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="7">
         <f>B7+((B4/2)/TAN(RADIANS(B6)))-2</f>
@@ -3138,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D816C7CA-793D-4BAF-98F3-443B8F117F52}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3152,7 +3158,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3173,10 +3179,27 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="4">
+        <f>SQRT(2)*Bulkhead!B7</f>
+        <v>70.569256762417453</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
Assembly fixes, added gear tooth profile to latches
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A8316F-6E7C-46BD-8B8F-18733AEED885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E974099-8D2D-4D13-8AA6-113279D2B8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" tabRatio="667" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="Shell" sheetId="7" r:id="rId4"/>
     <sheet name="Bulkhead" sheetId="8" r:id="rId5"/>
     <sheet name="Arm Wheel &amp; Arm" sheetId="11" r:id="rId6"/>
-    <sheet name="Electronics Board" sheetId="13" r:id="rId7"/>
+    <sheet name="Battery and Camera Holders" sheetId="13" r:id="rId7"/>
+    <sheet name="Nose Cone Release Gears" sheetId="15" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -330,6 +331,30 @@
   <si>
     <t>Offset from board</t>
   </si>
+  <si>
+    <t>Nose Cone Release Gears</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given by worm gear listing </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Pitch Diameter</t>
+  </si>
+  <si>
+    <t>Pressure Anngle</t>
+  </si>
+  <si>
+    <t>Shaft Diameter</t>
+  </si>
+  <si>
+    <t>Thread Starts</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +364,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +454,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -453,10 +486,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -491,11 +525,52 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -723,7 +798,7 @@
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{BF4FBE53-75C8-484D-9478-97DF7393A1CC}"/>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{677D2D52-0B6C-4B16-81C9-28445C0D9EA5}">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -786,8 +861,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5847D800-2737-4C4E-8650-CB8B550670C6}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B54988AB-35CD-4CE4-9584-860CA1529F9C}" name="Value" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{7F3F4D8D-127D-483C-A3C7-71EB956D9106}" name="Units" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{30BDBAD9-10CB-40CA-8069-09092D99504D}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -799,8 +874,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A9055BBA-1249-4E95-814E-26A0A5B1B66C}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DD9C9434-1260-4285-8F03-055DCA784D86}" name="Value" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{007F3DAB-D632-44E0-AF40-6A30D3CE697E}" name="Units" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{9C1D3036-3428-4217-BD9C-B256247B98EA}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -812,8 +887,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2AB09C10-555A-4FA5-825E-671C56C5204E}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{59C8A266-3FE0-4BD1-8096-042394DD0601}" name="Value" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{96950D65-C78A-461C-96D5-9CC3CC5987C0}" name="Units" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{7AF4781C-1A05-4414-BB69-E3894335BB8B}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -825,8 +900,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0B1EF6EA-7B8F-43FA-94CF-9EC466EA2E42}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{60F0019A-911A-4343-88C9-968557FAC235}" name="Value" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5E858251-C579-4557-A894-E703077E3D0B}" name="Units" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{59D44731-521A-4BFC-A838-854482140970}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -838,8 +913,8 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{08ED45E6-44A0-4E17-968F-5621C3E7B4A1}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{957D3AA8-B8AB-4AF6-865C-352EAE7F21BA}" name="Value" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{99CBAB39-6963-4DDA-B437-CB2F3F8008D2}" name="Units" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{957D3AA8-B8AB-4AF6-865C-352EAE7F21BA}" name="Value" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{99CBAB39-6963-4DDA-B437-CB2F3F8008D2}" name="Units" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{72EE9F42-A042-455C-9AEB-3FDF7CA75325}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -851,9 +926,22 @@
   <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{875DCB20-9A5B-4AE5-9B86-9FAA788CBC89}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{7B1A0CB3-1D6F-469F-9208-C86A05C85E0A}" name="Value" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{FB7EDCA0-CC79-4DF2-9D3C-281C141BCEF3}" name="Units" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7B1A0CB3-1D6F-469F-9208-C86A05C85E0A}" name="Value" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FB7EDCA0-CC79-4DF2-9D3C-281C141BCEF3}" name="Units" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{B19EAADD-84D4-408B-B3B0-38E4F735B850}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A6643120-A089-4129-B5E2-912677DE7807}" name="Table4234678" displayName="Table4234678" ref="A2:D1048576" totalsRowShown="0">
+  <autoFilter ref="A2:D1048576" xr:uid="{0F14B4B8-9B87-4941-AFFE-2D07ACC316B6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3D0BA2F2-EC74-4DE0-A9FE-E6F6B074AC4E}" name="Dimension"/>
+    <tableColumn id="2" xr3:uid="{2CC4207D-D21F-4020-BA6F-F9942E226649}" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8E9131FE-4543-4960-9103-F3E302FB6A56}" name="Units" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E4CB6C5D-981F-402A-91B2-5F2199D9741A}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3144,7 +3232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D816C7CA-793D-4BAF-98F3-443B8F117F52}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3439,4 +3527,344 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B03E3DA-7FE4-46D8-AA53-EFA49B8E0899}">
+  <dimension ref="A1:D80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="112.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="12">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="12">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="12">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{25213ED3-0F48-4A58-A772-E9AF5F8D5586}"/>
+    <hyperlink ref="D4:D7" r:id="rId2" display="Given by worm gear listing " xr:uid="{33A4EEA2-0DB9-4356-9A24-69D424D8F333}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added space for springs in nose cone, gerber files for PCB.
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E974099-8D2D-4D13-8AA6-113279D2B8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F752A295-7391-4EF4-8C50-CB2218DED1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" tabRatio="667" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -519,16 +519,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -948,9 +948,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -988,7 +988,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1094,7 +1094,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1236,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1264,54 +1264,54 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="11"/>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1670,12 +1670,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -1790,7 +1790,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>26</v>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="B12" s="7">
         <f>'Arm Wheel &amp; Arm'!B5+B11</f>
-        <v>6.2</v>
+        <v>8.5</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>26</v>
@@ -1813,7 +1813,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>26</v>
@@ -1896,12 +1896,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2252,12 +2252,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2562,12 +2562,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2900,8 +2900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414219C2-975E-4253-8115-B06CE1149AD2}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2913,12 +2913,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2961,7 +2961,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -3245,12 +3245,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3533,8 +3533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B03E3DA-7FE4-46D8-AA53-EFA49B8E0899}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3546,12 +3546,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3571,13 +3571,13 @@
       <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.8</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3591,7 +3591,7 @@
       <c r="C4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3605,7 +3605,7 @@
       <c r="C5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
       <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed mate spaghetti. Added flares to nose cone latches
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCAACBE-F75D-42B1-8DAB-64D301083765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654C45BB-8039-4153-96C6-601A08E85BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1942,7 +1942,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="1">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="B4" s="7">
         <f>Table42[[#This Row],[Value]]</f>
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated bulkhead thickness, new spacer stl's
</commit_message>
<xml_diff>
--- a/Working Model/model_design_dashboard.xlsx
+++ b/Working Model/model_design_dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\branigjg\Desktop\School\Capstone\Project-Crumple-Zone\Working Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greenac\Documents\Project-Crumple-Zone\Working Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654C45BB-8039-4153-96C6-601A08E85BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15EC456-D1D3-4EE2-8AB5-C1AFC1EC39E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="667" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Inputs" sheetId="3" r:id="rId1"/>
@@ -1892,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC87B61D-89B4-4354-BE4D-52F1AB79BE0D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2558,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F3E7A-7DA3-40B7-A994-AE85F749A01D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2620,7 +2620,8 @@
         <v>50</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <f>CONVERT(1/16,"in","mm")</f>
+        <v>1.5874999999999999</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>

</xml_diff>